<commit_message>
added c/p ratio option for shear strength.
</commit_message>
<xml_diff>
--- a/input_template.xlsx
+++ b/input_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njones/PycharmProjects/slopetools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB0F5F41-AA2A-D043-8DFA-37E84832F463}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9485FA8E-B5EB-9845-BEB9-526B8B9BB297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20780" yWindow="940" windowWidth="32160" windowHeight="24340" xr2:uid="{BA54C293-CE08-6E4C-9212-B3317DAA148E}"/>
+    <workbookView xWindow="32780" yWindow="760" windowWidth="32160" windowHeight="24340" activeTab="3" xr2:uid="{BA54C293-CE08-6E4C-9212-B3317DAA148E}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="109">
   <si>
     <t>X</t>
   </si>
@@ -420,6 +420,50 @@
   </si>
   <si>
     <t>SlopeTools Input Template</t>
+  </si>
+  <si>
+    <t>option</t>
+  </si>
+  <si>
+    <t>mc</t>
+  </si>
+  <si>
+    <t>Strength options</t>
+  </si>
+  <si>
+    <t>Traditional Mohr-Coulomb failure envelope (c and phi)</t>
+  </si>
+  <si>
+    <t>cp</t>
+  </si>
+  <si>
+    <t>c/p ratio with reference elevation</t>
+  </si>
+  <si>
+    <t>r-elev</t>
+  </si>
+  <si>
+    <t>c/p</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="0"/>
+        <rFont val="Symbol"/>
+        <charset val="2"/>
+      </rPr>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="0"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(c/p)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -623,7 +667,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -680,6 +724,9 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -701,14 +748,99 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="11">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -4298,7 +4430,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D02E090B-D957-7046-AD33-44E170F709C1}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -4327,10 +4459,10 @@
       <c r="C5" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="24"/>
+      <c r="E5" s="25"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
@@ -4339,10 +4471,10 @@
       <c r="C6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="22"/>
+      <c r="E6" s="23"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
@@ -4351,10 +4483,10 @@
       <c r="C7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="22"/>
+      <c r="E7" s="23"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
@@ -4363,10 +4495,10 @@
       <c r="C8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="22"/>
+      <c r="E8" s="23"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
@@ -4375,10 +4507,10 @@
       <c r="C9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="D9" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="22"/>
+      <c r="E9" s="23"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
@@ -4387,10 +4519,10 @@
       <c r="C10" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="22" t="s">
+      <c r="D10" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="E10" s="22"/>
+      <c r="E10" s="23"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
@@ -4399,10 +4531,10 @@
       <c r="C11" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="D11" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="22"/>
+      <c r="E11" s="23"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
@@ -4411,10 +4543,10 @@
       <c r="C12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="22" t="s">
+      <c r="D12" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="E12" s="22"/>
+      <c r="E12" s="23"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B13" s="1"/>
@@ -4423,11 +4555,11 @@
       <c r="B14" s="1"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C16" s="15" t="s">
@@ -4515,26 +4647,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="D2" s="25" t="s">
+      <c r="B2" s="26"/>
+      <c r="D2" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="25"/>
-      <c r="G2" s="25" t="s">
+      <c r="E2" s="26"/>
+      <c r="G2" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="25"/>
-      <c r="J2" s="25" t="s">
+      <c r="H2" s="26"/>
+      <c r="J2" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="25"/>
-      <c r="M2" s="25" t="s">
+      <c r="K2" s="26"/>
+      <c r="M2" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="25"/>
+      <c r="N2" s="26"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -4781,26 +4913,26 @@
       <c r="N18" s="3"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20" s="25" t="s">
+      <c r="A20" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="25"/>
-      <c r="D20" s="25" t="s">
+      <c r="B20" s="26"/>
+      <c r="D20" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="E20" s="25"/>
-      <c r="G20" s="25" t="s">
+      <c r="E20" s="26"/>
+      <c r="G20" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="H20" s="25"/>
-      <c r="J20" s="25" t="s">
+      <c r="H20" s="26"/>
+      <c r="J20" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="K20" s="25"/>
-      <c r="M20" s="25" t="s">
+      <c r="K20" s="26"/>
+      <c r="M20" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="N20" s="25"/>
+      <c r="N20" s="26"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
@@ -5016,16 +5148,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="M20:N20"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="M20:N20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5033,34 +5165,39 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAA88A0E-2BF5-FE49-9603-08BE4D91829B}">
-  <dimension ref="A2:K13"/>
+  <dimension ref="A2:O13"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="10.83203125" style="1"/>
-    <col min="6" max="8" width="11.1640625" customWidth="1"/>
+    <col min="1" max="1" width="7" style="1" customWidth="1"/>
+    <col min="2" max="8" width="8.5" style="1" customWidth="1"/>
+    <col min="9" max="12" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B2" s="26" t="s">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B2" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="F2" s="26" t="s">
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="I2" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="J2" t="s">
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="22"/>
+      <c r="N2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>14</v>
       </c>
@@ -5068,100 +5205,134 @@
         <v>83</v>
       </c>
       <c r="C3" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="E3" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="H3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="I3" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="J3" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="K3" s="17" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L3" s="6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>1</v>
       </c>
       <c r="B4" s="3">
         <v>130</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" s="3">
         <v>200</v>
       </c>
-      <c r="D4" s="3">
+      <c r="E4" s="3">
         <v>28</v>
       </c>
-      <c r="E4" s="3">
+      <c r="F4" s="3">
+        <v>30</v>
+      </c>
+      <c r="G4" s="3">
+        <v>120</v>
+      </c>
+      <c r="H4" s="3">
         <v>1</v>
       </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="J4" s="7" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="N4" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>2</v>
       </c>
       <c r="B5" s="3">
         <v>120</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D5" s="3">
         <v>100</v>
       </c>
-      <c r="D5" s="3">
+      <c r="E5" s="3">
         <v>32</v>
-      </c>
-      <c r="E5" s="3">
-        <v>1</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="J5" s="1">
-        <v>0</v>
-      </c>
-      <c r="K5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H5" s="3">
+        <v>1</v>
+      </c>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="N5" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="O5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>3</v>
       </c>
       <c r="B6" s="3">
         <v>132</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D6" s="3">
         <v>400</v>
       </c>
-      <c r="D6" s="3">
+      <c r="E6" s="3">
         <v>27</v>
-      </c>
-      <c r="E6" s="3">
-        <v>1</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="J6" s="1">
+      <c r="H6" s="3">
         <v>1</v>
       </c>
-      <c r="K6" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="N6" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="O6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>4</v>
       </c>
@@ -5172,8 +5343,12 @@
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>5</v>
       </c>
@@ -5184,8 +5359,15 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="N8" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>6</v>
       </c>
@@ -5196,9 +5378,18 @@
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
-      <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="N9" s="1">
+        <v>0</v>
+      </c>
+      <c r="O9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>7</v>
       </c>
@@ -5209,9 +5400,18 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
-      <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="N10" s="1">
+        <v>1</v>
+      </c>
+      <c r="O10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>8</v>
       </c>
@@ -5222,9 +5422,13 @@
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
-      <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="N11" s="1"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>9</v>
       </c>
@@ -5235,9 +5439,13 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
-      <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="N12" s="1"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>10</v>
       </c>
@@ -5248,15 +5456,41 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="F2:H2"/>
+  <mergeCells count="1">
+    <mergeCell ref="B2:G2"/>
   </mergeCells>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4:E13" xr:uid="{339A18D9-2C3F-2E47-9927-C099D7AA59DB}">
-      <formula1>$J$5:$J$6</formula1>
+  <conditionalFormatting sqref="D4:E13">
+    <cfRule type="expression" dxfId="9" priority="5">
+      <formula>$C4="cp"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F4:G13">
+    <cfRule type="expression" dxfId="8" priority="4">
+      <formula>$C4="mc"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L4:L13">
+    <cfRule type="expression" dxfId="7" priority="3">
+      <formula>$C4="mc"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J4:K13">
+    <cfRule type="expression" dxfId="6" priority="1">
+      <formula>$C4="cp"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4:H13" xr:uid="{339A18D9-2C3F-2E47-9927-C099D7AA59DB}">
+      <formula1>$N$9:$N$10</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C13" xr:uid="{D6CE31A3-485A-D842-BAD0-54ACE6AD61ED}">
+      <formula1>$N$5:$N$6</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5274,10 +5508,10 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="27"/>
+      <c r="B2" s="28"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -5461,7 +5695,6 @@
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
-      <c r="I5" s="29"/>
       <c r="J5" s="1" t="s">
         <v>32</v>
       </c>
@@ -5480,7 +5713,6 @@
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
-      <c r="I6" s="29"/>
       <c r="J6" s="1" t="s">
         <v>38</v>
       </c>
@@ -5499,7 +5731,6 @@
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
-      <c r="I7" s="29"/>
       <c r="J7" s="1" t="s">
         <v>96</v>
       </c>
@@ -5518,7 +5749,6 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
-      <c r="I8" s="29"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
@@ -5531,7 +5761,6 @@
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
-      <c r="I9" s="29"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
@@ -5544,7 +5773,6 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
-      <c r="I10" s="29"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
@@ -5557,7 +5785,6 @@
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
-      <c r="I11" s="29"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
@@ -5570,7 +5797,6 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
-      <c r="I12" s="29"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
@@ -5583,7 +5809,6 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
-      <c r="I13" s="29"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
@@ -5596,7 +5821,6 @@
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
-      <c r="I14" s="29"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -5782,26 +6006,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="F2" s="28" t="s">
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="F2" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="J2" s="28" t="s">
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="J2" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="N2" s="28" t="s">
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="N2" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="O2" s="28"/>
-      <c r="P2" s="28"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
@@ -5994,26 +6218,26 @@
       <c r="P13" s="3"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="F15" s="28" t="s">
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="F15" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="J15" s="28" t="s">
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="J15" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="K15" s="28"/>
-      <c r="L15" s="28"/>
-      <c r="N15" s="28" t="s">
+      <c r="K15" s="29"/>
+      <c r="L15" s="29"/>
+      <c r="N15" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="O15" s="28"/>
-      <c r="P15" s="28"/>
+      <c r="O15" s="29"/>
+      <c r="P15" s="29"/>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
@@ -6230,30 +6454,30 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="G2" s="28" t="s">
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="G2" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="L2" s="28" t="s">
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="L2" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="28"/>
-      <c r="Q2" s="28" t="s">
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="Q2" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="R2" s="28"/>
-      <c r="S2" s="28"/>
-      <c r="T2" s="28"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="29"/>
     </row>
     <row r="3" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
@@ -6620,30 +6844,30 @@
       <c r="T13" s="3"/>
     </row>
     <row r="15" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="G15" s="28" t="s">
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="G15" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
-      <c r="L15" s="28" t="s">
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="29"/>
+      <c r="L15" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="M15" s="28"/>
-      <c r="N15" s="28"/>
-      <c r="O15" s="28"/>
-      <c r="Q15" s="28" t="s">
+      <c r="M15" s="29"/>
+      <c r="N15" s="29"/>
+      <c r="O15" s="29"/>
+      <c r="Q15" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="R15" s="28"/>
-      <c r="S15" s="28"/>
-      <c r="T15" s="28"/>
+      <c r="R15" s="29"/>
+      <c r="S15" s="29"/>
+      <c r="T15" s="29"/>
     </row>
     <row r="16" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
@@ -6876,30 +7100,30 @@
       <c r="T26" s="3"/>
     </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B28" s="28" t="s">
+      <c r="B28" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="C28" s="28"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
-      <c r="G28" s="28" t="s">
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="G28" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="H28" s="28"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="28"/>
-      <c r="L28" s="28" t="s">
+      <c r="H28" s="29"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="29"/>
+      <c r="L28" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="M28" s="28"/>
-      <c r="N28" s="28"/>
-      <c r="O28" s="28"/>
-      <c r="Q28" s="28" t="s">
+      <c r="M28" s="29"/>
+      <c r="N28" s="29"/>
+      <c r="O28" s="29"/>
+      <c r="Q28" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="R28" s="28"/>
-      <c r="S28" s="28"/>
-      <c r="T28" s="28"/>
+      <c r="R28" s="29"/>
+      <c r="S28" s="29"/>
+      <c r="T28" s="29"/>
     </row>
     <row r="29" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B29" s="2" t="s">

</xml_diff>

<commit_message>
distributed loads and plotting
</commit_message>
<xml_diff>
--- a/input_template.xlsx
+++ b/input_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njones/PycharmProjects/slopetools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9485FA8E-B5EB-9845-BEB9-526B8B9BB297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBA983CD-D4FE-594F-8472-DE7BE8B328F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32780" yWindow="760" windowWidth="32160" windowHeight="24340" activeTab="3" xr2:uid="{BA54C293-CE08-6E4C-9212-B3317DAA148E}"/>
+    <workbookView xWindow="32780" yWindow="760" windowWidth="32160" windowHeight="24340" activeTab="7" xr2:uid="{BA54C293-CE08-6E4C-9212-B3317DAA148E}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -727,6 +727,7 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -748,19 +749,15 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="4">
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor theme="2" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
     </dxf>
@@ -781,62 +778,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4459,10 +4401,10 @@
       <c r="C5" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="25"/>
+      <c r="E5" s="26"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
@@ -4471,10 +4413,10 @@
       <c r="C6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="23"/>
+      <c r="E6" s="24"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
@@ -4483,10 +4425,10 @@
       <c r="C7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D7" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="23"/>
+      <c r="E7" s="24"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
@@ -4495,10 +4437,10 @@
       <c r="C8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D8" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="23"/>
+      <c r="E8" s="24"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
@@ -4507,10 +4449,10 @@
       <c r="C9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="23" t="s">
+      <c r="D9" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="23"/>
+      <c r="E9" s="24"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
@@ -4519,10 +4461,10 @@
       <c r="C10" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="23" t="s">
+      <c r="D10" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="E10" s="23"/>
+      <c r="E10" s="24"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
@@ -4531,10 +4473,10 @@
       <c r="C11" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="23" t="s">
+      <c r="D11" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="23"/>
+      <c r="E11" s="24"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
@@ -4543,10 +4485,10 @@
       <c r="C12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="23" t="s">
+      <c r="D12" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="E12" s="23"/>
+      <c r="E12" s="24"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B13" s="1"/>
@@ -4555,11 +4497,11 @@
       <c r="B14" s="1"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C16" s="15" t="s">
@@ -4647,26 +4589,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="D2" s="26" t="s">
+      <c r="B2" s="27"/>
+      <c r="D2" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="26"/>
-      <c r="G2" s="26" t="s">
+      <c r="E2" s="27"/>
+      <c r="G2" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="26"/>
-      <c r="J2" s="26" t="s">
+      <c r="H2" s="27"/>
+      <c r="J2" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="26"/>
-      <c r="M2" s="26" t="s">
+      <c r="K2" s="27"/>
+      <c r="M2" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="26"/>
+      <c r="N2" s="27"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -4913,26 +4855,26 @@
       <c r="N18" s="3"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20" s="26" t="s">
+      <c r="A20" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="26"/>
-      <c r="D20" s="26" t="s">
+      <c r="B20" s="27"/>
+      <c r="D20" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="E20" s="26"/>
-      <c r="G20" s="26" t="s">
+      <c r="E20" s="27"/>
+      <c r="G20" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="H20" s="26"/>
-      <c r="J20" s="26" t="s">
+      <c r="H20" s="27"/>
+      <c r="J20" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="K20" s="26"/>
-      <c r="M20" s="26" t="s">
+      <c r="K20" s="27"/>
+      <c r="M20" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="N20" s="26"/>
+      <c r="N20" s="27"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
@@ -5148,16 +5090,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="M2:N2"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="G20:H20"/>
     <mergeCell ref="J20:K20"/>
     <mergeCell ref="M20:N20"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="M2:N2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5167,7 +5109,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAA88A0E-2BF5-FE49-9603-08BE4D91829B}">
   <dimension ref="A2:O13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
@@ -5179,19 +5121,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="I2" s="30" t="s">
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="I2" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
       <c r="L2" s="22"/>
       <c r="N2" t="s">
         <v>90</v>
@@ -5466,23 +5408,23 @@
     <mergeCell ref="B2:G2"/>
   </mergeCells>
   <conditionalFormatting sqref="D4:E13">
-    <cfRule type="expression" dxfId="9" priority="5">
+    <cfRule type="expression" dxfId="3" priority="5">
       <formula>$C4="cp"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4:G13">
-    <cfRule type="expression" dxfId="8" priority="4">
-      <formula>$C4="mc"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L4:L13">
-    <cfRule type="expression" dxfId="7" priority="3">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>$C4="mc"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:K13">
-    <cfRule type="expression" dxfId="6" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>$C4="cp"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L4:L13">
+    <cfRule type="expression" dxfId="0" priority="3">
+      <formula>$C4="mc"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
@@ -5508,10 +5450,10 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="28"/>
+      <c r="B2" s="29"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -5989,8 +5931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7976BB56-7732-404C-B58A-55DA7F8052B3}">
   <dimension ref="B2:P26"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6006,26 +5948,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="F2" s="29" t="s">
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="F2" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="J2" s="29" t="s">
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="J2" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="N2" s="29" t="s">
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="N2" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="O2" s="29"/>
-      <c r="P2" s="29"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
@@ -6073,7 +6015,7 @@
         <v>84</v>
       </c>
       <c r="D4" s="3">
-        <v>500</v>
+        <v>2500</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -6093,7 +6035,7 @@
         <v>84</v>
       </c>
       <c r="D5" s="3">
-        <v>500</v>
+        <v>2500</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -6218,26 +6160,26 @@
       <c r="P13" s="3"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="F15" s="29" t="s">
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="F15" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="G15" s="29"/>
-      <c r="H15" s="29"/>
-      <c r="J15" s="29" t="s">
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="J15" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="K15" s="29"/>
-      <c r="L15" s="29"/>
-      <c r="N15" s="29" t="s">
+      <c r="K15" s="30"/>
+      <c r="L15" s="30"/>
+      <c r="N15" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="O15" s="29"/>
-      <c r="P15" s="29"/>
+      <c r="O15" s="30"/>
+      <c r="P15" s="30"/>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
@@ -6454,30 +6396,30 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="G2" s="29" t="s">
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="G2" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="L2" s="29" t="s">
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="L2" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
-      <c r="O2" s="29"/>
-      <c r="Q2" s="29" t="s">
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="Q2" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="R2" s="29"/>
-      <c r="S2" s="29"/>
-      <c r="T2" s="29"/>
+      <c r="R2" s="30"/>
+      <c r="S2" s="30"/>
+      <c r="T2" s="30"/>
     </row>
     <row r="3" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
@@ -6844,30 +6786,30 @@
       <c r="T13" s="3"/>
     </row>
     <row r="15" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="G15" s="29" t="s">
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="G15" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="H15" s="29"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="29"/>
-      <c r="L15" s="29" t="s">
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
+      <c r="L15" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="M15" s="29"/>
-      <c r="N15" s="29"/>
-      <c r="O15" s="29"/>
-      <c r="Q15" s="29" t="s">
+      <c r="M15" s="30"/>
+      <c r="N15" s="30"/>
+      <c r="O15" s="30"/>
+      <c r="Q15" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="R15" s="29"/>
-      <c r="S15" s="29"/>
-      <c r="T15" s="29"/>
+      <c r="R15" s="30"/>
+      <c r="S15" s="30"/>
+      <c r="T15" s="30"/>
     </row>
     <row r="16" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
@@ -7100,30 +7042,30 @@
       <c r="T26" s="3"/>
     </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B28" s="29" t="s">
+      <c r="B28" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="G28" s="29" t="s">
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30"/>
+      <c r="G28" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="H28" s="29"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="29"/>
-      <c r="L28" s="29" t="s">
+      <c r="H28" s="30"/>
+      <c r="I28" s="30"/>
+      <c r="J28" s="30"/>
+      <c r="L28" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="M28" s="29"/>
-      <c r="N28" s="29"/>
-      <c r="O28" s="29"/>
-      <c r="Q28" s="29" t="s">
+      <c r="M28" s="30"/>
+      <c r="N28" s="30"/>
+      <c r="O28" s="30"/>
+      <c r="Q28" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="R28" s="29"/>
-      <c r="S28" s="29"/>
-      <c r="T28" s="29"/>
+      <c r="R28" s="30"/>
+      <c r="S28" s="30"/>
+      <c r="T28" s="30"/>
     </row>
     <row r="29" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B29" s="2" t="s">

</xml_diff>

<commit_message>
Added non-circular surface option
</commit_message>
<xml_diff>
--- a/input_template.xlsx
+++ b/input_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njones/PycharmProjects/slopetools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBA983CD-D4FE-594F-8472-DE7BE8B328F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E4F9BC-FCE4-1743-8139-CF62ED3B7E2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32780" yWindow="760" windowWidth="32160" windowHeight="24340" activeTab="7" xr2:uid="{BA54C293-CE08-6E4C-9212-B3317DAA148E}"/>
+    <workbookView xWindow="12660" yWindow="1220" windowWidth="32160" windowHeight="24340" activeTab="1" xr2:uid="{BA54C293-CE08-6E4C-9212-B3317DAA148E}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -1692,10 +1692,10 @@
                   <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>40</c:v>
@@ -4556,7 +4556,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56CEDAD3-D805-AE4D-9F0D-9E80BF51FF21}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
@@ -5090,16 +5090,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="M20:N20"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="M20:N20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5779,7 +5779,7 @@
   <dimension ref="A2:F17"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5828,7 +5828,7 @@
         <v>100</v>
       </c>
       <c r="B4" s="3">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>48</v>
@@ -5845,7 +5845,7 @@
         <v>220</v>
       </c>
       <c r="B5" s="3">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>48</v>
@@ -5931,7 +5931,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7976BB56-7732-404C-B58A-55DA7F8052B3}">
   <dimension ref="B2:P26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Tried to get Spencer's to work and failed.
</commit_message>
<xml_diff>
--- a/input_template.xlsx
+++ b/input_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njones/PycharmProjects/slopetools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E4F9BC-FCE4-1743-8139-CF62ED3B7E2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8543402D-81BD-D540-8CA7-368B8E7A5FFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12660" yWindow="1220" windowWidth="32160" windowHeight="24340" activeTab="1" xr2:uid="{BA54C293-CE08-6E4C-9212-B3317DAA148E}"/>
   </bookViews>
@@ -1677,7 +1677,7 @@
                   <c:v>220</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>250</c:v>
+                  <c:v>240</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5779,7 +5779,7 @@
   <dimension ref="A2:F17"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5853,7 +5853,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="B6" s="3">
         <v>40</v>

</xml_diff>